<commit_message>
Added W43 as outlier
</commit_message>
<xml_diff>
--- a/outlier_summary.xlsx
+++ b/outlier_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="278" documentId="8_{A80B4BEF-9EE6-41C1-9D10-5036FAC1EACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DD1ACC9-59CE-41B3-9423-DD886FA9D6C2}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="8_{A80B4BEF-9EE6-41C1-9D10-5036FAC1EACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D74CC33-A021-4747-8BC0-FAA1C676E2C6}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{96D4777A-9411-461B-AF8E-5FB3803EAFD8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96D4777A-9411-461B-AF8E-5FB3803EAFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
   <si>
     <t>Metric</t>
   </si>
@@ -150,9 +150,6 @@
     <t>SlopeTime</t>
   </si>
   <si>
-    <t>S49</t>
-  </si>
-  <si>
     <t>P22</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
   </si>
   <si>
     <t>W44</t>
-  </si>
-  <si>
-    <t>SlopeTime, DNA</t>
   </si>
   <si>
     <t>S47</t>
@@ -181,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +187,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,10 +225,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,20 +544,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A134AA89-A0E1-4B86-A7E7-7C8B9EF223C9}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -575,7 +577,7 @@
         <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
@@ -605,7 +607,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -640,7 +642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -675,7 +677,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -719,7 +721,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -757,45 +759,51 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>8.4700833000000006</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>-29.09</v>
       </c>
-      <c r="H6">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
         <v>4172</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>2</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>4064</v>
       </c>
-      <c r="L6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6">
+      <c r="L6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="1">
         <v>157.19999999999999</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <v>37</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="1">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -841,7 +849,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -876,7 +884,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -911,7 +919,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -946,7 +954,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -981,7 +989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1013,7 +1021,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1045,7 +1053,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1077,7 +1085,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1109,123 +1117,123 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I19" t="s">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20">
+        <v>56.837577269999997</v>
+      </c>
+      <c r="H20">
+        <v>3982</v>
+      </c>
+      <c r="I20" t="s">
         <v>14</v>
       </c>
-      <c r="J19">
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>3961</v>
+      </c>
+      <c r="L20" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20">
+        <v>158</v>
+      </c>
+      <c r="N20">
+        <v>35</v>
+      </c>
+      <c r="O20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="3">
+        <v>181.68805750000001</v>
+      </c>
+      <c r="H21" s="3">
+        <v>4173</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="3">
         <v>2</v>
       </c>
-      <c r="K19">
-        <v>4076</v>
-      </c>
-      <c r="L19" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19">
-        <v>147.6</v>
-      </c>
-      <c r="N19">
-        <v>33</v>
-      </c>
-      <c r="O19">
+      <c r="K21" s="3">
+        <v>4064</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="3">
+        <v>110.3</v>
+      </c>
+      <c r="N21" s="3">
+        <v>36.5</v>
+      </c>
+      <c r="O21" s="3">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="3">
+        <v>171.78411389999999</v>
+      </c>
+      <c r="H22" s="3">
+        <v>4126</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>4065</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="3">
+        <v>162</v>
+      </c>
+      <c r="N22" s="3">
+        <v>36</v>
+      </c>
+      <c r="O22" s="3">
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20">
-        <v>3.1669999999999998</v>
-      </c>
-      <c r="G20">
-        <v>10.08733518</v>
-      </c>
-      <c r="H20">
-        <v>4108</v>
-      </c>
-      <c r="I20" t="s">
-        <v>40</v>
-      </c>
-      <c r="J20">
-        <v>2</v>
-      </c>
-      <c r="K20">
-        <v>4066</v>
-      </c>
-      <c r="L20" t="s">
-        <v>11</v>
-      </c>
-      <c r="M20">
-        <v>111.4</v>
-      </c>
-      <c r="N20">
-        <v>39</v>
-      </c>
-      <c r="O20">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22">
-        <v>56.837577269999997</v>
-      </c>
-      <c r="H22">
-        <v>3982</v>
-      </c>
-      <c r="I22" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="K22">
-        <v>3961</v>
-      </c>
-      <c r="L22" t="s">
-        <v>11</v>
-      </c>
-      <c r="M22">
-        <v>158</v>
-      </c>
-      <c r="N22">
-        <v>35</v>
-      </c>
-      <c r="O22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
       <c r="G23">
-        <v>181.68805750000001</v>
+        <v>101.1179403</v>
       </c>
       <c r="H23">
-        <v>4173</v>
+        <v>4130</v>
       </c>
       <c r="I23" t="s">
         <v>10</v>
@@ -1234,89 +1242,57 @@
         <v>2</v>
       </c>
       <c r="K23">
-        <v>4064</v>
+        <v>4073</v>
       </c>
       <c r="L23" t="s">
         <v>11</v>
       </c>
       <c r="M23">
-        <v>110.3</v>
+        <v>149.80000000000001</v>
       </c>
       <c r="N23">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="O23">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+      <c r="F24">
+        <v>3.1669999999999998</v>
       </c>
       <c r="G24">
-        <v>171.78411389999999</v>
+        <v>10.08733518</v>
       </c>
       <c r="H24">
-        <v>4126</v>
+        <v>4108</v>
       </c>
       <c r="I24" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="J24">
         <v>2</v>
       </c>
       <c r="K24">
-        <v>4065</v>
+        <v>4066</v>
       </c>
       <c r="L24" t="s">
         <v>11</v>
       </c>
       <c r="M24">
-        <v>162</v>
+        <v>111.4</v>
       </c>
       <c r="N24">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="O24">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25">
-        <v>101.1179403</v>
-      </c>
-      <c r="H25">
-        <v>4130</v>
-      </c>
-      <c r="I25" t="s">
-        <v>10</v>
-      </c>
-      <c r="J25">
-        <v>2</v>
-      </c>
-      <c r="K25">
-        <v>4073</v>
-      </c>
-      <c r="L25" t="s">
-        <v>11</v>
-      </c>
-      <c r="M25">
-        <v>149.80000000000001</v>
-      </c>
-      <c r="N25">
-        <v>36</v>
-      </c>
-      <c r="O25">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated w/ additional d metrics; tested baseline against Season x ABX x Diet x Substrate
</commit_message>
<xml_diff>
--- a/outlier_summary.xlsx
+++ b/outlier_summary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="288" documentId="8_{A80B4BEF-9EE6-41C1-9D10-5036FAC1EACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D74CC33-A021-4747-8BC0-FAA1C676E2C6}"/>
+  <xr:revisionPtr revIDLastSave="548" documentId="8_{A80B4BEF-9EE6-41C1-9D10-5036FAC1EACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0434B3D3-6B79-4CDF-9FBB-3DECE16FAF17}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96D4777A-9411-461B-AF8E-5FB3803EAFD8}"/>
+    <workbookView xWindow="-432" yWindow="4248" windowWidth="13716" windowHeight="5340" activeTab="1" xr2:uid="{96D4777A-9411-461B-AF8E-5FB3803EAFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="66">
   <si>
     <t>Metric</t>
   </si>
@@ -169,13 +170,76 @@
   </si>
   <si>
     <t>P20</t>
+  </si>
+  <si>
+    <t>ABX?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>AUC Big</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>AUC Low</t>
+  </si>
+  <si>
+    <t>W36</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>W32</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Lower than ABX squirrels</t>
+  </si>
+  <si>
+    <t>Higher than No ABX squirrels</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Higher than no ABX</t>
+  </si>
+  <si>
+    <t>MaxD</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>P41</t>
+  </si>
+  <si>
+    <t>DNA Yield</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>Highest ABX DNA yield</t>
+  </si>
+  <si>
+    <t>P05, P06 (high); P24(low)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,8 +262,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +287,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,11 +309,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A134AA89-A0E1-4B86-A7E7-7C8B9EF223C9}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1299,4 +1387,870 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60103D9C-593D-4380-9FAF-5BAA7C0DB149}">
+  <dimension ref="A1:R45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>6563.8977999999997</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5">
+        <v>960.45609999999999</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5">
+        <v>212.66159999999999</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="5">
+        <v>8.3283334</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8.4700833000000006</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4">
+        <v>-60.027500099999997</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6">
+        <v>-18.71</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="6">
+        <v>-28.82</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>-26.83</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <v>-26.1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6">
+        <v>-23.77</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="7">
+        <v>-60.027500099999997</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F14" s="7">
+        <v>-28.6533333</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="7">
+        <v>8.4700833000000006</v>
+      </c>
+      <c r="D15" s="6">
+        <v>-29.09</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5">
+        <v>82.023529999999994</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5">
+        <v>323.86667</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5">
+        <v>31.84</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5">
+        <v>15.48</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5">
+        <v>10.1</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>391.69666999999998</v>
+      </c>
+      <c r="H24" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25">
+        <v>65.513329999999996</v>
+      </c>
+      <c r="H25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="H26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4">
+        <v>-28.6533333</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5">
+        <v>5.1433333000000001</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4">
+        <v>-28.82</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1">
+        <v>-26.46</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5">
+        <v>-23.77</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4">
+        <v>-29.09</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35">
+        <v>-26.83</v>
+      </c>
+      <c r="H35" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37">
+        <v>56.837577269999997</v>
+      </c>
+      <c r="H37" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38">
+        <v>181.68805750000001</v>
+      </c>
+      <c r="H38" t="s">
+        <v>46</v>
+      </c>
+      <c r="I38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39">
+        <v>10.08733518</v>
+      </c>
+      <c r="H39" t="s">
+        <v>49</v>
+      </c>
+      <c r="I39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="G40">
+        <v>171.78411389999999</v>
+      </c>
+      <c r="H40" t="s">
+        <v>46</v>
+      </c>
+      <c r="I40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="G41">
+        <v>101.1179403</v>
+      </c>
+      <c r="H41" t="s">
+        <v>49</v>
+      </c>
+      <c r="I41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43">
+        <v>181.68806000000001</v>
+      </c>
+      <c r="H43" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G44">
+        <v>10.08733518</v>
+      </c>
+      <c r="H44" t="s">
+        <v>49</v>
+      </c>
+      <c r="I44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="G45">
+        <v>56.837577269999997</v>
+      </c>
+      <c r="H45" t="s">
+        <v>49</v>
+      </c>
+      <c r="I45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with outliers removed
</commit_message>
<xml_diff>
--- a/outlier_summary.xlsx
+++ b/outlier_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="717" documentId="8_{A80B4BEF-9EE6-41C1-9D10-5036FAC1EACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2A09255-6EC1-48D8-B6FB-954706E42553}"/>
+  <xr:revisionPtr revIDLastSave="752" documentId="8_{A80B4BEF-9EE6-41C1-9D10-5036FAC1EACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A655C8E5-6A7D-47ED-B430-A62420609182}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{96D4777A-9411-461B-AF8E-5FB3803EAFD8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="87">
   <si>
     <t>Metric</t>
   </si>
@@ -263,9 +263,6 @@
     <t>Low baseline, high MaxD, AUC higher than No ABX</t>
   </si>
   <si>
-    <t>Just very effective ABX?</t>
-  </si>
-  <si>
     <t>ABX didn't work well?</t>
   </si>
   <si>
@@ -281,13 +278,25 @@
     <t>Crazy increase after 2 hr --&gt; check notes</t>
   </si>
   <si>
-    <t>Check notes. Pretty steady</t>
-  </si>
-  <si>
     <t>Increases after hour 2</t>
   </si>
   <si>
     <t>Even when you take the one other baseline measurement, its baseline is still an outlier</t>
+  </si>
+  <si>
+    <t>It has 1 other baseline measurement that's still way low</t>
+  </si>
+  <si>
+    <t>No water bottle records. When its 3 baseline measurements are averaged, that avg baseline isn't an outlier so I'm using that as the baseline instead</t>
+  </si>
+  <si>
+    <t>When its 3 baseline measurements are averaged, that avg baseline isn't an outlier so I'm using that avg baseline instead</t>
+  </si>
+  <si>
+    <t>Other 2 baselines were even lower. Avg baseline is still outlier</t>
+  </si>
+  <si>
+    <t>Avg baseline is still outlier</t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -411,7 +420,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -2241,10 +2249,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2985BA97-5B4E-4187-854A-C6188D89FFFD}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2305,135 +2313,11 @@
         <v>33</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10">
-        <v>-28.82</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="R2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="15">
-        <v>16.513300000000001</v>
-      </c>
-      <c r="D3" s="15">
-        <v>-27.22</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15">
-        <v>65.513329999999996</v>
-      </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15">
-        <v>-23.77</v>
-      </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9">
-        <v>8.2763270000000002</v>
-      </c>
-      <c r="D5" s="10">
-        <v>-29.09</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10">
-        <v>5.1433333000000001</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
@@ -2449,85 +2333,6 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="16">
-        <v>31.94501</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16">
-        <v>391.69666999999998</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="16">
-        <v>8.2677589999999999</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16">
-        <v>18.760000000000002</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16">
-        <v>22.064308069999999</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
@@ -2570,7 +2375,7 @@
         <v>34</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -2590,7 +2395,9 @@
       <c r="F18" s="13">
         <v>3186.7467000000001</v>
       </c>
-      <c r="G18" s="13"/>
+      <c r="G18" s="13">
+        <v>56.837577269999997</v>
+      </c>
       <c r="H18" s="13" t="s">
         <v>49</v>
       </c>
@@ -2609,7 +2416,7 @@
         <v>34</v>
       </c>
       <c r="S18" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -2638,50 +2445,277 @@
       <c r="R19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="S19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="9">
+        <v>8.2763270000000002</v>
+      </c>
+      <c r="D20" s="10">
+        <v>-29.09</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10">
+        <v>5.1433333000000001</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="S20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14">
+        <v>-23.77</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="10"/>
+      <c r="S21" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12">
         <v>785.53663400000005</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="11" t="s">
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I23" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B24" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3">
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12">
         <v>-2.4666667000000002</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="14" t="s">
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I24" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J24" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11">
+        <v>22.064308069999999</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J25" s="11" t="s">
         <v>79</v>
+      </c>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="11">
+        <v>8.2677589999999999</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="11">
+        <v>31.94501</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11">
+        <v>391.69666999999998</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10">
+        <v>-28.82</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="R28" t="s">
+        <v>34</v>
+      </c>
+      <c r="S28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="14">
+        <v>16.513300000000001</v>
+      </c>
+      <c r="D29" s="14">
+        <v>-27.22</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14">
+        <v>65.513329999999996</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="S29" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DNA yield outlier check for ABX squirrels; started abx plots
</commit_message>
<xml_diff>
--- a/outlier_summary.xlsx
+++ b/outlier_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="752" documentId="8_{A80B4BEF-9EE6-41C1-9D10-5036FAC1EACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A655C8E5-6A7D-47ED-B430-A62420609182}"/>
+  <xr:revisionPtr revIDLastSave="759" documentId="8_{A80B4BEF-9EE6-41C1-9D10-5036FAC1EACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46509736-A759-48CE-8D16-4260EFFEEFC9}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{96D4777A-9411-461B-AF8E-5FB3803EAFD8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{96D4777A-9411-461B-AF8E-5FB3803EAFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="88">
   <si>
     <t>Metric</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Avg baseline is still outlier</t>
+  </si>
+  <si>
+    <t>DNA yield</t>
   </si>
 </sst>
 </file>
@@ -2252,7 +2255,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2316,7 +2319,29 @@
         <v>76</v>
       </c>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
       <c r="L4" s="10"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>